<commit_message>
Sletta kolonner fra Shi-excel-fila.
</commit_message>
<xml_diff>
--- a/Shi_20.xlsx
+++ b/Shi_20.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23115"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitetetitromso.sharepoint.com/sites/O365-Flippedclassroomreview/Shared Documents/Publication Bias/Exceldatafiler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tla005\Documents\RStudio_Projects\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_E2208EDC8AB81AB19E8826932F6DFD4B08BC7E9C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0B4F11-AB7E-48AA-8F1B-867E9DFE0A0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="8895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shi et al 2020" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Study </t>
   </si>
@@ -54,15 +54,6 @@
   </si>
   <si>
     <t>n2i</t>
-  </si>
-  <si>
-    <t>SMD</t>
-  </si>
-  <si>
-    <t>LL</t>
-  </si>
-  <si>
-    <t>UL</t>
   </si>
   <si>
     <t>Asiksoy &amp; Ozdamil (2016)</t>
@@ -168,7 +159,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,18 +479,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -521,19 +510,10 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
       <c r="B2">
         <v>74.63</v>
@@ -553,19 +533,10 @@
       <c r="G2">
         <v>30</v>
       </c>
-      <c r="H2">
-        <v>5.08</v>
-      </c>
-      <c r="I2">
-        <v>4.07</v>
-      </c>
-      <c r="J2">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>84.1</v>
@@ -585,19 +556,10 @@
       <c r="G3">
         <v>362</v>
       </c>
-      <c r="H3">
-        <v>0.6</v>
-      </c>
-      <c r="I3">
-        <v>0.46</v>
-      </c>
-      <c r="J3">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>74</v>
@@ -617,19 +579,10 @@
       <c r="G4">
         <v>24</v>
       </c>
-      <c r="H4">
-        <v>0.47</v>
-      </c>
-      <c r="I4">
-        <v>-0.12</v>
-      </c>
-      <c r="J4">
-        <v>1.07</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>83.12</v>
@@ -649,19 +602,10 @@
       <c r="G5">
         <v>23</v>
       </c>
-      <c r="H5">
-        <v>0.97</v>
-      </c>
-      <c r="I5">
-        <v>0.3</v>
-      </c>
-      <c r="J5">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>80.2</v>
@@ -681,19 +625,10 @@
       <c r="G6">
         <v>56</v>
       </c>
-      <c r="H6">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="I6">
-        <v>0.77</v>
-      </c>
-      <c r="J6">
-        <v>1.51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>88.3</v>
@@ -713,19 +648,10 @@
       <c r="G7">
         <v>165</v>
       </c>
-      <c r="H7">
-        <v>0.4</v>
-      </c>
-      <c r="I7">
-        <v>0.18</v>
-      </c>
-      <c r="J7">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>74.66</v>
@@ -745,19 +671,10 @@
       <c r="G8">
         <v>371</v>
       </c>
-      <c r="H8">
-        <v>0.78</v>
-      </c>
-      <c r="I8">
-        <v>0.64</v>
-      </c>
-      <c r="J8">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>73.599999999999994</v>
@@ -777,19 +694,10 @@
       <c r="G9">
         <v>294</v>
       </c>
-      <c r="H9">
-        <v>-0.02</v>
-      </c>
-      <c r="I9">
-        <v>-0.17</v>
-      </c>
-      <c r="J9">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>71.489999999999995</v>
@@ -809,19 +717,10 @@
       <c r="G10">
         <v>20</v>
       </c>
-      <c r="H10">
-        <v>1.8</v>
-      </c>
-      <c r="I10">
-        <v>1.08</v>
-      </c>
-      <c r="J10">
-        <v>2.52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>91.35</v>
@@ -841,19 +740,10 @@
       <c r="G11">
         <v>75</v>
       </c>
-      <c r="H11">
-        <v>0.03</v>
-      </c>
-      <c r="I11">
-        <v>-0.28999999999999998</v>
-      </c>
-      <c r="J11">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>76.8</v>
@@ -873,19 +763,10 @@
       <c r="G12">
         <v>34</v>
       </c>
-      <c r="H12">
-        <v>0.82</v>
-      </c>
-      <c r="I12">
-        <v>0.32</v>
-      </c>
-      <c r="J12">
-        <v>1.33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>43.9</v>
@@ -905,19 +786,10 @@
       <c r="G13">
         <v>343</v>
       </c>
-      <c r="H13">
-        <v>0.12</v>
-      </c>
-      <c r="I13">
-        <v>-0.03</v>
-      </c>
-      <c r="J13">
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>71</v>
@@ -937,19 +809,10 @@
       <c r="G14">
         <v>30</v>
       </c>
-      <c r="H14">
-        <v>0.51</v>
-      </c>
-      <c r="I14">
-        <v>0.05</v>
-      </c>
-      <c r="J14">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>77.819999999999993</v>
@@ -969,19 +832,10 @@
       <c r="G15">
         <v>71</v>
       </c>
-      <c r="H15">
-        <v>0.15</v>
-      </c>
-      <c r="I15">
-        <v>-0.18</v>
-      </c>
-      <c r="J15">
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>83.31</v>
@@ -1001,19 +855,10 @@
       <c r="G16">
         <v>25</v>
       </c>
-      <c r="H16">
-        <v>1.52</v>
-      </c>
-      <c r="I16">
-        <v>0.89</v>
-      </c>
-      <c r="J16">
-        <v>2.14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>78.5</v>
@@ -1033,19 +878,10 @@
       <c r="G17">
         <v>76</v>
       </c>
-      <c r="H17">
-        <v>-0.11</v>
-      </c>
-      <c r="I17">
-        <v>-0.43</v>
-      </c>
-      <c r="J17">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>67.290000000000006</v>
@@ -1065,19 +901,10 @@
       <c r="G18">
         <v>100</v>
       </c>
-      <c r="H18">
-        <v>-0.01</v>
-      </c>
-      <c r="I18">
-        <v>-0.25</v>
-      </c>
-      <c r="J18">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>84.41</v>
@@ -1097,19 +924,10 @@
       <c r="G19">
         <v>25</v>
       </c>
-      <c r="H19">
-        <v>2.04</v>
-      </c>
-      <c r="I19">
-        <v>1.33</v>
-      </c>
-      <c r="J19">
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>62.39</v>
@@ -1129,19 +947,10 @@
       <c r="G20">
         <v>18</v>
       </c>
-      <c r="H20">
-        <v>-0.84</v>
-      </c>
-      <c r="I20">
-        <v>-1.5</v>
-      </c>
-      <c r="J20">
-        <v>-0.17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>74.75</v>
@@ -1161,19 +970,10 @@
       <c r="G21">
         <v>92</v>
       </c>
-      <c r="H21">
-        <v>-0.12</v>
-      </c>
-      <c r="I21">
-        <v>-0.41</v>
-      </c>
-      <c r="J21">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>64.81</v>
@@ -1193,19 +993,10 @@
       <c r="G22">
         <v>244</v>
       </c>
-      <c r="H22">
-        <v>0.39</v>
-      </c>
-      <c r="I22">
-        <v>0.23</v>
-      </c>
-      <c r="J22">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>79</v>
@@ -1225,19 +1016,10 @@
       <c r="G23">
         <v>101</v>
       </c>
-      <c r="H23">
-        <v>-0.27</v>
-      </c>
-      <c r="I23">
-        <v>-0.54</v>
-      </c>
-      <c r="J23">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24">
         <v>56.06</v>
@@ -1257,19 +1039,10 @@
       <c r="G24">
         <v>120</v>
       </c>
-      <c r="H24">
-        <v>0.4</v>
-      </c>
-      <c r="I24">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J24">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>64</v>
@@ -1289,19 +1062,10 @@
       <c r="G25">
         <v>25</v>
       </c>
-      <c r="H25">
-        <v>0.67</v>
-      </c>
-      <c r="I25">
-        <v>0.1</v>
-      </c>
-      <c r="J25">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>82.3</v>
@@ -1321,19 +1085,10 @@
       <c r="G26">
         <v>19</v>
       </c>
-      <c r="H26">
-        <v>0.73</v>
-      </c>
-      <c r="I26">
-        <v>0.11</v>
-      </c>
-      <c r="J26">
-        <v>1.35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>61.63</v>
@@ -1353,19 +1108,10 @@
       <c r="G27">
         <v>175</v>
       </c>
-      <c r="H27">
-        <v>0.01</v>
-      </c>
-      <c r="I27">
-        <v>-0.24</v>
-      </c>
-      <c r="J27">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B28">
         <v>51.4</v>
@@ -1385,19 +1131,10 @@
       <c r="G28">
         <v>55</v>
       </c>
-      <c r="H28">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="I28">
-        <v>0.15</v>
-      </c>
-      <c r="J28">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B29">
         <v>69.09</v>
@@ -1417,19 +1154,10 @@
       <c r="G29">
         <v>90</v>
       </c>
-      <c r="H29">
-        <v>0.45</v>
-      </c>
-      <c r="I29">
-        <v>0.16</v>
-      </c>
-      <c r="J29">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>68</v>
@@ -1449,19 +1177,10 @@
       <c r="G30">
         <v>14</v>
       </c>
-      <c r="H30">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I30">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="J30">
-        <v>1.92</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B31">
         <v>73.790000000000006</v>
@@ -1481,19 +1200,10 @@
       <c r="G31">
         <v>77</v>
       </c>
-      <c r="H31">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I31">
-        <v>-0.04</v>
-      </c>
-      <c r="J31">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B32">
         <v>83.8</v>
@@ -1513,19 +1223,10 @@
       <c r="G32">
         <v>58</v>
       </c>
-      <c r="H32">
-        <v>0.26</v>
-      </c>
-      <c r="I32">
-        <v>-0.11</v>
-      </c>
-      <c r="J32">
-        <v>0.62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B33">
         <v>71.77</v>
@@ -1545,19 +1246,10 @@
       <c r="G33">
         <v>25</v>
       </c>
-      <c r="H33">
-        <v>0.99</v>
-      </c>
-      <c r="I33">
-        <v>0.46</v>
-      </c>
-      <c r="J33">
-        <v>1.53</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B34">
         <v>76.430000000000007</v>
@@ -1576,15 +1268,6 @@
       </c>
       <c r="G34">
         <v>36</v>
-      </c>
-      <c r="H34">
-        <v>0.5</v>
-      </c>
-      <c r="I34">
-        <v>0.02</v>
-      </c>
-      <c r="J34">
-        <v>0.97</v>
       </c>
     </row>
   </sheetData>
@@ -1594,6 +1277,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AC21DF0D7558742B677ED624C9CEB1E" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48155dd33cb802efe448fb61149a0a6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8a1c249-5d44-4dec-a049-9454fa097088" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d644393cea86b1a490953364ee2c840f" ns2:_="">
     <xsd:import namespace="f8a1c249-5d44-4dec-a049-9454fa097088"/>
@@ -1771,29 +1469,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F615BACC-9702-48BD-9764-39D4CEBC2864}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{505AD628-33E3-4FC6-9BF2-22C25AA751AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D518D1B-2D07-45F7-8F4A-752D7383CD53}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D518D1B-2D07-45F7-8F4A-752D7383CD53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{505AD628-33E3-4FC6-9BF2-22C25AA751AB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F615BACC-9702-48BD-9764-39D4CEBC2864}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f8a1c249-5d44-4dec-a049-9454fa097088"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Endret navn fra method til design på moderator 2
</commit_message>
<xml_diff>
--- a/Shi_20.xlsx
+++ b/Shi_20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rgs022\Documents\R\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C48CEAEB-D272-4DFA-B9D0-7014D3A44C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C13D87-7568-4DF8-9C06-1E951DE9B4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13890" yWindow="-15645" windowWidth="14400" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shi et al 2020" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>n2i</t>
   </si>
   <si>
-    <t>method</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>Cotta et al.</t>
+  </si>
+  <si>
+    <t>design</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,10 +501,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -525,12 +525,12 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2">
         <v>2016</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>2016</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>2017</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2">
         <v>2017</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2">
         <v>2015</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2">
         <v>2016</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2">
         <v>2017</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2">
         <v>2016</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2">
         <v>2017</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2">
         <v>2017</v>
@@ -817,7 +817,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="2">
         <v>2016</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2">
         <v>2016</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="2">
         <v>2017</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="2">
         <v>2016</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2">
         <v>2015</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2">
         <v>2015</v>
@@ -991,7 +991,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2">
         <v>2014</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2">
         <v>2017</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2">
         <v>2017</v>
@@ -1078,7 +1078,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2">
         <v>2016</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2">
         <v>2016</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2">
         <v>2017</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2">
         <v>2016</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2">
         <v>2016</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" s="2">
         <v>2016</v>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2">
         <v>2016</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="2">
         <v>2016</v>
@@ -1310,7 +1310,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2">
         <v>2016</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="2">
         <v>2013</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="2">
         <v>2017</v>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B32" s="2">
         <v>2015</v>
@@ -1426,7 +1426,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="2">
         <v>2016</v>
@@ -1455,7 +1455,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B34" s="2">
         <v>2016</v>
@@ -1495,15 +1495,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AC21DF0D7558742B677ED624C9CEB1E" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48155dd33cb802efe448fb61149a0a6b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8a1c249-5d44-4dec-a049-9454fa097088" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d644393cea86b1a490953364ee2c840f" ns2:_="">
     <xsd:import namespace="f8a1c249-5d44-4dec-a049-9454fa097088"/>
@@ -1681,6 +1672,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D518D1B-2D07-45F7-8F4A-752D7383CD53}">
   <ds:schemaRefs>
@@ -1698,14 +1698,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{505AD628-33E3-4FC6-9BF2-22C25AA751AB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F615BACC-9702-48BD-9764-39D4CEBC2864}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1721,4 +1713,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{505AD628-33E3-4FC6-9BF2-22C25AA751AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>